<commit_message>
update on repo for permission management
</commit_message>
<xml_diff>
--- a/Portal/wwwroot/SalesReport.xlsx
+++ b/Portal/wwwroot/SalesReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t xml:space="preserve">12000.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARM StockTrade: Online stock trading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Securities</t>
   </si>
   <si>
     <t xml:space="preserve">2019-01-29 15:04:48</t>
@@ -148,21 +154,61 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Several Changes made to the Client Portal.
</commit_message>
<xml_diff>
--- a/Portal/wwwroot/SalesReport.xlsx
+++ b/Portal/wwwroot/SalesReport.xlsx
@@ -6,13 +6,13 @@
     <workbookView tabRatio="600"/>
   </bookViews>
   <sheets>
-    <sheet name="Demo" sheetId="1" r:id="rId3"/>
+    <sheet name="AllTime" sheetId="1" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -32,34 +32,58 @@
     <t xml:space="preserve">Amount</t>
   </si>
   <si>
-    <t xml:space="preserve">2019-01-29 15:04:51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EF7CD7A436C5439292AEF58D2287C4F2</t>
+    <t xml:space="preserve">Feb 21 2019  8:27AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100000008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesica Micheal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARM Money Market Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mutual Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1300.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34000.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb 21 2019  7:43AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100000007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb 21 2019  7:30AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100000005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosy John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2300.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb 21 2019  7:24AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100000002</t>
   </si>
   <si>
     <t xml:space="preserve">Alic John</t>
   </si>
   <si>
-    <t xml:space="preserve">ARM Discovery Fund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mutual Fund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12000.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARM StockTrade: Online stock trading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Securities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-01-29 15:04:48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12DEF2A916614EE8BC7CB905F4AABE13</t>
+    <t xml:space="preserve">5000.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100000001</t>
   </si>
   <si>
     <t xml:space="preserve">Mark John</t>
@@ -163,30 +187,30 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -194,22 +218,82 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>